<commit_message>
Fix package run warnings.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-VIEWSS/MS-VIEWSS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-VIEWSS/MS-VIEWSS_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -3944,9 +3944,6 @@
     <t>MS-VIEWSS_R8005001</t>
   </si>
   <si>
-    <t>MS-VIEWSS_R8005:I; MS-VIEWSS_R148:i</t>
-  </si>
-  <si>
     <t>Verified by requirements: MS-VIEWSS_R8014, MS-VIEWSS_R8005001.</t>
   </si>
   <si>
@@ -3960,12 +3957,15 @@
   </si>
   <si>
     <t>Verified by requirement: MS-VIEWSS_R8902001.</t>
+  </si>
+  <si>
+    <t>MS-VIEWSS_R8005:i, MS-VIEWSS_R148:i</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -4231,21 +4231,6 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4270,55 +4255,26 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4657,6 +4613,50 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4786,34 +4786,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I378" tableType="xml" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I378" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I378"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="24">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="23">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="22">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="21">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="20">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="19">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="18">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="17">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="16">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -4822,12 +4822,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="10"/>
-    <tableColumn id="2" name="Test" dataDxfId="9"/>
-    <tableColumn id="3" name="Description" dataDxfId="8"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4876,7 +4876,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4909,9 +4909,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4944,6 +4961,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5123,21 +5157,19 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD54"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="11" width="9" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9" style="3"/>
   </cols>
@@ -5179,127 +5211,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -5312,12 +5344,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -5330,12 +5362,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -5348,12 +5380,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -5366,60 +5398,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -5478,7 +5510,7 @@
       </c>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="21" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A21" s="22" t="s">
         <v>44</v>
       </c>
@@ -5580,7 +5612,7 @@
       </c>
       <c r="I24" s="24"/>
     </row>
-    <row r="25" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="25" spans="1:12" s="23" customFormat="1">
       <c r="A25" s="22" t="s">
         <v>48</v>
       </c>
@@ -5655,7 +5687,7 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="60">
+    <row r="28" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A28" s="22" t="s">
         <v>51</v>
       </c>
@@ -5880,7 +5912,7 @@
       </c>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:9" ht="30">
+    <row r="37" spans="1:9">
       <c r="A37" s="30" t="s">
         <v>60</v>
       </c>
@@ -6105,7 +6137,7 @@
       </c>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" spans="1:9" ht="135">
+    <row r="46" spans="1:9" ht="120">
       <c r="A46" s="30" t="s">
         <v>69</v>
       </c>
@@ -6130,7 +6162,7 @@
       </c>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" spans="1:9" ht="45">
+    <row r="47" spans="1:9" ht="30">
       <c r="A47" s="30" t="s">
         <v>70</v>
       </c>
@@ -6180,7 +6212,7 @@
       </c>
       <c r="I48" s="32"/>
     </row>
-    <row r="49" spans="1:9" ht="135">
+    <row r="49" spans="1:9" ht="120">
       <c r="A49" s="30" t="s">
         <v>72</v>
       </c>
@@ -6205,7 +6237,7 @@
       </c>
       <c r="I49" s="32"/>
     </row>
-    <row r="50" spans="1:9" ht="45">
+    <row r="50" spans="1:9" ht="30">
       <c r="A50" s="30" t="s">
         <v>73</v>
       </c>
@@ -6330,7 +6362,7 @@
       </c>
       <c r="I54" s="32"/>
     </row>
-    <row r="55" spans="1:9" ht="30">
+    <row r="55" spans="1:9">
       <c r="A55" s="30" t="s">
         <v>78</v>
       </c>
@@ -6430,7 +6462,7 @@
       </c>
       <c r="I58" s="32"/>
     </row>
-    <row r="59" spans="1:9" ht="135">
+    <row r="59" spans="1:9" ht="120">
       <c r="A59" s="30" t="s">
         <v>82</v>
       </c>
@@ -6455,7 +6487,7 @@
       </c>
       <c r="I59" s="32"/>
     </row>
-    <row r="60" spans="1:9" ht="45">
+    <row r="60" spans="1:9" ht="30">
       <c r="A60" s="30" t="s">
         <v>83</v>
       </c>
@@ -6655,7 +6687,7 @@
       </c>
       <c r="I67" s="32"/>
     </row>
-    <row r="68" spans="1:9" ht="45">
+    <row r="68" spans="1:9" ht="30">
       <c r="A68" s="30" t="s">
         <v>91</v>
       </c>
@@ -6734,7 +6766,7 @@
       </c>
       <c r="I70" s="32"/>
     </row>
-    <row r="71" spans="1:9" ht="30">
+    <row r="71" spans="1:9">
       <c r="A71" s="30" t="s">
         <v>94</v>
       </c>
@@ -6784,7 +6816,7 @@
       </c>
       <c r="I72" s="32"/>
     </row>
-    <row r="73" spans="1:9" ht="135">
+    <row r="73" spans="1:9" ht="120">
       <c r="A73" s="30" t="s">
         <v>96</v>
       </c>
@@ -6834,7 +6866,7 @@
       </c>
       <c r="I74" s="32"/>
     </row>
-    <row r="75" spans="1:9" ht="60">
+    <row r="75" spans="1:9" ht="45">
       <c r="A75" s="30" t="s">
         <v>98</v>
       </c>
@@ -7059,7 +7091,7 @@
       </c>
       <c r="I83" s="32"/>
     </row>
-    <row r="84" spans="1:9" ht="30">
+    <row r="84" spans="1:9">
       <c r="A84" s="30" t="s">
         <v>107</v>
       </c>
@@ -7184,7 +7216,7 @@
       </c>
       <c r="I88" s="32"/>
     </row>
-    <row r="89" spans="1:9" ht="30">
+    <row r="89" spans="1:9">
       <c r="A89" s="30" t="s">
         <v>112</v>
       </c>
@@ -7234,7 +7266,7 @@
       </c>
       <c r="I90" s="32"/>
     </row>
-    <row r="91" spans="1:9" ht="30">
+    <row r="91" spans="1:9">
       <c r="A91" s="30" t="s">
         <v>114</v>
       </c>
@@ -7284,7 +7316,7 @@
       </c>
       <c r="I92" s="32"/>
     </row>
-    <row r="93" spans="1:9" ht="30">
+    <row r="93" spans="1:9">
       <c r="A93" s="30" t="s">
         <v>116</v>
       </c>
@@ -7459,7 +7491,7 @@
       </c>
       <c r="I99" s="32"/>
     </row>
-    <row r="100" spans="1:9" ht="30">
+    <row r="100" spans="1:9">
       <c r="A100" s="30" t="s">
         <v>123</v>
       </c>
@@ -7484,7 +7516,7 @@
       </c>
       <c r="I100" s="32"/>
     </row>
-    <row r="101" spans="1:9" ht="30">
+    <row r="101" spans="1:9">
       <c r="A101" s="30" t="s">
         <v>124</v>
       </c>
@@ -7509,7 +7541,7 @@
       </c>
       <c r="I101" s="32"/>
     </row>
-    <row r="102" spans="1:9" ht="45">
+    <row r="102" spans="1:9" ht="30">
       <c r="A102" s="30" t="s">
         <v>125</v>
       </c>
@@ -7584,7 +7616,7 @@
       </c>
       <c r="I104" s="32"/>
     </row>
-    <row r="105" spans="1:9" ht="120">
+    <row r="105" spans="1:9" ht="105">
       <c r="A105" s="30" t="s">
         <v>128</v>
       </c>
@@ -7784,7 +7816,7 @@
       </c>
       <c r="I112" s="32"/>
     </row>
-    <row r="113" spans="1:9" ht="60">
+    <row r="113" spans="1:9" ht="45">
       <c r="A113" s="30" t="s">
         <v>135</v>
       </c>
@@ -7811,7 +7843,7 @@
       </c>
       <c r="I113" s="32"/>
     </row>
-    <row r="114" spans="1:9" ht="60">
+    <row r="114" spans="1:9" ht="45">
       <c r="A114" s="30" t="s">
         <v>136</v>
       </c>
@@ -7819,7 +7851,7 @@
         <v>415</v>
       </c>
       <c r="C114" s="32" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="D114" s="30" t="s">
         <v>828</v>
@@ -7837,10 +7869,10 @@
         <v>17</v>
       </c>
       <c r="I114" s="32" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" ht="30">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
       <c r="A115" s="30" t="s">
         <v>137</v>
       </c>
@@ -7865,7 +7897,7 @@
       </c>
       <c r="I115" s="32"/>
     </row>
-    <row r="116" spans="1:9" ht="30">
+    <row r="116" spans="1:9">
       <c r="A116" s="30" t="s">
         <v>138</v>
       </c>
@@ -7940,7 +7972,7 @@
       </c>
       <c r="I118" s="32"/>
     </row>
-    <row r="119" spans="1:9" ht="45">
+    <row r="119" spans="1:9" ht="30">
       <c r="A119" s="30" t="s">
         <v>141</v>
       </c>
@@ -7965,7 +7997,7 @@
       </c>
       <c r="I119" s="32"/>
     </row>
-    <row r="120" spans="1:9" ht="45">
+    <row r="120" spans="1:9" ht="30">
       <c r="A120" s="30" t="s">
         <v>142</v>
       </c>
@@ -8040,7 +8072,7 @@
       </c>
       <c r="I122" s="32"/>
     </row>
-    <row r="123" spans="1:9" ht="30">
+    <row r="123" spans="1:9">
       <c r="A123" s="30" t="s">
         <v>145</v>
       </c>
@@ -8290,7 +8322,7 @@
       </c>
       <c r="I132" s="32"/>
     </row>
-    <row r="133" spans="1:9" ht="45">
+    <row r="133" spans="1:9" ht="30">
       <c r="A133" s="30" t="s">
         <v>155</v>
       </c>
@@ -8315,7 +8347,7 @@
       </c>
       <c r="I133" s="32"/>
     </row>
-    <row r="134" spans="1:9" ht="30">
+    <row r="134" spans="1:9">
       <c r="A134" s="30" t="s">
         <v>156</v>
       </c>
@@ -8340,7 +8372,7 @@
       </c>
       <c r="I134" s="32"/>
     </row>
-    <row r="135" spans="1:9" ht="30">
+    <row r="135" spans="1:9">
       <c r="A135" s="30" t="s">
         <v>157</v>
       </c>
@@ -8390,7 +8422,7 @@
       </c>
       <c r="I136" s="32"/>
     </row>
-    <row r="137" spans="1:9" ht="30">
+    <row r="137" spans="1:9">
       <c r="A137" s="30" t="s">
         <v>159</v>
       </c>
@@ -8415,7 +8447,7 @@
       </c>
       <c r="I137" s="32"/>
     </row>
-    <row r="138" spans="1:9" ht="30">
+    <row r="138" spans="1:9">
       <c r="A138" s="30" t="s">
         <v>160</v>
       </c>
@@ -8440,7 +8472,7 @@
       </c>
       <c r="I138" s="32"/>
     </row>
-    <row r="139" spans="1:9" ht="30">
+    <row r="139" spans="1:9">
       <c r="A139" s="30" t="s">
         <v>161</v>
       </c>
@@ -8815,7 +8847,7 @@
       </c>
       <c r="I153" s="32"/>
     </row>
-    <row r="154" spans="1:9" ht="30">
+    <row r="154" spans="1:9">
       <c r="A154" s="30" t="s">
         <v>174</v>
       </c>
@@ -9148,7 +9180,7 @@
       </c>
       <c r="I166" s="32"/>
     </row>
-    <row r="167" spans="1:9" ht="30">
+    <row r="167" spans="1:9">
       <c r="A167" s="30" t="s">
         <v>187</v>
       </c>
@@ -9202,7 +9234,7 @@
       </c>
       <c r="I168" s="32"/>
     </row>
-    <row r="169" spans="1:9" ht="45">
+    <row r="169" spans="1:9" ht="30">
       <c r="A169" s="30" t="s">
         <v>189</v>
       </c>
@@ -9252,7 +9284,7 @@
       </c>
       <c r="I170" s="32"/>
     </row>
-    <row r="171" spans="1:9" ht="225">
+    <row r="171" spans="1:9" ht="210">
       <c r="A171" s="30" t="s">
         <v>191</v>
       </c>
@@ -9351,7 +9383,7 @@
         <v>17</v>
       </c>
       <c r="I174" s="32" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="30">
@@ -9379,7 +9411,7 @@
       </c>
       <c r="I175" s="32"/>
     </row>
-    <row r="176" spans="1:9" ht="30">
+    <row r="176" spans="1:9">
       <c r="A176" s="30" t="s">
         <v>196</v>
       </c>
@@ -9429,7 +9461,7 @@
       </c>
       <c r="I177" s="32"/>
     </row>
-    <row r="178" spans="1:9" ht="45">
+    <row r="178" spans="1:9" ht="30">
       <c r="A178" s="30" t="s">
         <v>198</v>
       </c>
@@ -9454,7 +9486,7 @@
       </c>
       <c r="I178" s="32"/>
     </row>
-    <row r="179" spans="1:9" ht="30">
+    <row r="179" spans="1:9">
       <c r="A179" s="30" t="s">
         <v>199</v>
       </c>
@@ -9479,7 +9511,7 @@
       </c>
       <c r="I179" s="32"/>
     </row>
-    <row r="180" spans="1:9" ht="30">
+    <row r="180" spans="1:9">
       <c r="A180" s="30" t="s">
         <v>200</v>
       </c>
@@ -9554,7 +9586,7 @@
       </c>
       <c r="I182" s="32"/>
     </row>
-    <row r="183" spans="1:9" ht="30">
+    <row r="183" spans="1:9">
       <c r="A183" s="30" t="s">
         <v>203</v>
       </c>
@@ -9579,7 +9611,7 @@
       </c>
       <c r="I183" s="32"/>
     </row>
-    <row r="184" spans="1:9" ht="30">
+    <row r="184" spans="1:9">
       <c r="A184" s="30" t="s">
         <v>204</v>
       </c>
@@ -9604,7 +9636,7 @@
       </c>
       <c r="I184" s="32"/>
     </row>
-    <row r="185" spans="1:9" ht="30">
+    <row r="185" spans="1:9">
       <c r="A185" s="30" t="s">
         <v>205</v>
       </c>
@@ -9854,7 +9886,7 @@
       </c>
       <c r="I194" s="32"/>
     </row>
-    <row r="195" spans="1:9" ht="45">
+    <row r="195" spans="1:9" ht="30">
       <c r="A195" s="30" t="s">
         <v>215</v>
       </c>
@@ -9879,7 +9911,7 @@
       </c>
       <c r="I195" s="32"/>
     </row>
-    <row r="196" spans="1:9" ht="30">
+    <row r="196" spans="1:9">
       <c r="A196" s="30" t="s">
         <v>216</v>
       </c>
@@ -9904,7 +9936,7 @@
       </c>
       <c r="I196" s="32"/>
     </row>
-    <row r="197" spans="1:9" ht="30">
+    <row r="197" spans="1:9">
       <c r="A197" s="30" t="s">
         <v>217</v>
       </c>
@@ -9979,7 +10011,7 @@
       </c>
       <c r="I199" s="32"/>
     </row>
-    <row r="200" spans="1:9" ht="30">
+    <row r="200" spans="1:9">
       <c r="A200" s="30" t="s">
         <v>220</v>
       </c>
@@ -10004,7 +10036,7 @@
       </c>
       <c r="I200" s="32"/>
     </row>
-    <row r="201" spans="1:9" ht="30">
+    <row r="201" spans="1:9">
       <c r="A201" s="30" t="s">
         <v>221</v>
       </c>
@@ -10029,7 +10061,7 @@
       </c>
       <c r="I201" s="32"/>
     </row>
-    <row r="202" spans="1:9" ht="30">
+    <row r="202" spans="1:9">
       <c r="A202" s="30" t="s">
         <v>222</v>
       </c>
@@ -10054,7 +10086,7 @@
       </c>
       <c r="I202" s="32"/>
     </row>
-    <row r="203" spans="1:9" ht="30">
+    <row r="203" spans="1:9">
       <c r="A203" s="30" t="s">
         <v>223</v>
       </c>
@@ -10179,7 +10211,7 @@
       </c>
       <c r="I207" s="32"/>
     </row>
-    <row r="208" spans="1:9" ht="225">
+    <row r="208" spans="1:9" ht="210">
       <c r="A208" s="30" t="s">
         <v>228</v>
       </c>
@@ -10229,7 +10261,7 @@
       </c>
       <c r="I209" s="32"/>
     </row>
-    <row r="210" spans="1:9" ht="45">
+    <row r="210" spans="1:9" ht="30">
       <c r="A210" s="30" t="s">
         <v>230</v>
       </c>
@@ -10354,7 +10386,7 @@
       </c>
       <c r="I214" s="32"/>
     </row>
-    <row r="215" spans="1:9" ht="30">
+    <row r="215" spans="1:9">
       <c r="A215" s="30" t="s">
         <v>235</v>
       </c>
@@ -10429,7 +10461,7 @@
       </c>
       <c r="I217" s="32"/>
     </row>
-    <row r="218" spans="1:9" ht="30">
+    <row r="218" spans="1:9">
       <c r="A218" s="30" t="s">
         <v>238</v>
       </c>
@@ -10629,7 +10661,7 @@
       </c>
       <c r="I225" s="32"/>
     </row>
-    <row r="226" spans="1:9" ht="375">
+    <row r="226" spans="1:9" ht="360">
       <c r="A226" s="30" t="s">
         <v>246</v>
       </c>
@@ -10654,7 +10686,7 @@
       </c>
       <c r="I226" s="32"/>
     </row>
-    <row r="227" spans="1:9" ht="30">
+    <row r="227" spans="1:9">
       <c r="A227" s="30" t="s">
         <v>247</v>
       </c>
@@ -10679,7 +10711,7 @@
       </c>
       <c r="I227" s="32"/>
     </row>
-    <row r="228" spans="1:9" ht="45">
+    <row r="228" spans="1:9" ht="30">
       <c r="A228" s="30" t="s">
         <v>248</v>
       </c>
@@ -10704,7 +10736,7 @@
       </c>
       <c r="I228" s="32"/>
     </row>
-    <row r="229" spans="1:9" ht="45">
+    <row r="229" spans="1:9" ht="30">
       <c r="A229" s="30" t="s">
         <v>249</v>
       </c>
@@ -10779,7 +10811,7 @@
       </c>
       <c r="I231" s="32"/>
     </row>
-    <row r="232" spans="1:9" ht="45">
+    <row r="232" spans="1:9" ht="30">
       <c r="A232" s="30" t="s">
         <v>252</v>
       </c>
@@ -10804,7 +10836,7 @@
       </c>
       <c r="I232" s="32"/>
     </row>
-    <row r="233" spans="1:9" ht="30">
+    <row r="233" spans="1:9">
       <c r="A233" s="30" t="s">
         <v>253</v>
       </c>
@@ -10829,7 +10861,7 @@
       </c>
       <c r="I233" s="32"/>
     </row>
-    <row r="234" spans="1:9" ht="30">
+    <row r="234" spans="1:9">
       <c r="A234" s="30" t="s">
         <v>254</v>
       </c>
@@ -10879,7 +10911,7 @@
       </c>
       <c r="I235" s="32"/>
     </row>
-    <row r="236" spans="1:9" ht="30">
+    <row r="236" spans="1:9">
       <c r="A236" s="30" t="s">
         <v>256</v>
       </c>
@@ -10904,7 +10936,7 @@
       </c>
       <c r="I236" s="32"/>
     </row>
-    <row r="237" spans="1:9" ht="30">
+    <row r="237" spans="1:9">
       <c r="A237" s="30" t="s">
         <v>257</v>
       </c>
@@ -10929,7 +10961,7 @@
       </c>
       <c r="I237" s="32"/>
     </row>
-    <row r="238" spans="1:9" ht="30">
+    <row r="238" spans="1:9">
       <c r="A238" s="30" t="s">
         <v>258</v>
       </c>
@@ -10954,7 +10986,7 @@
       </c>
       <c r="I238" s="32"/>
     </row>
-    <row r="239" spans="1:9" ht="30">
+    <row r="239" spans="1:9">
       <c r="A239" s="30" t="s">
         <v>259</v>
       </c>
@@ -11104,7 +11136,7 @@
       </c>
       <c r="I244" s="32"/>
     </row>
-    <row r="245" spans="1:9" ht="240">
+    <row r="245" spans="1:9" ht="210">
       <c r="A245" s="30" t="s">
         <v>265</v>
       </c>
@@ -11179,7 +11211,7 @@
       </c>
       <c r="I247" s="32"/>
     </row>
-    <row r="248" spans="1:9" ht="30">
+    <row r="248" spans="1:9">
       <c r="A248" s="30" t="s">
         <v>268</v>
       </c>
@@ -11254,7 +11286,7 @@
       </c>
       <c r="I250" s="32"/>
     </row>
-    <row r="251" spans="1:9" ht="45">
+    <row r="251" spans="1:9" ht="30">
       <c r="A251" s="30" t="s">
         <v>271</v>
       </c>
@@ -11279,7 +11311,7 @@
       </c>
       <c r="I251" s="32"/>
     </row>
-    <row r="252" spans="1:9" ht="30">
+    <row r="252" spans="1:9">
       <c r="A252" s="30" t="s">
         <v>272</v>
       </c>
@@ -11304,7 +11336,7 @@
       </c>
       <c r="I252" s="32"/>
     </row>
-    <row r="253" spans="1:9" ht="30">
+    <row r="253" spans="1:9">
       <c r="A253" s="30" t="s">
         <v>273</v>
       </c>
@@ -11354,7 +11386,7 @@
       </c>
       <c r="I254" s="32"/>
     </row>
-    <row r="255" spans="1:9" ht="30">
+    <row r="255" spans="1:9">
       <c r="A255" s="30" t="s">
         <v>275</v>
       </c>
@@ -11379,7 +11411,7 @@
       </c>
       <c r="I255" s="32"/>
     </row>
-    <row r="256" spans="1:9" ht="30">
+    <row r="256" spans="1:9">
       <c r="A256" s="30" t="s">
         <v>276</v>
       </c>
@@ -11404,7 +11436,7 @@
       </c>
       <c r="I256" s="32"/>
     </row>
-    <row r="257" spans="1:9" ht="30">
+    <row r="257" spans="1:9">
       <c r="A257" s="30" t="s">
         <v>277</v>
       </c>
@@ -11429,7 +11461,7 @@
       </c>
       <c r="I257" s="32"/>
     </row>
-    <row r="258" spans="1:9" ht="30">
+    <row r="258" spans="1:9">
       <c r="A258" s="30" t="s">
         <v>278</v>
       </c>
@@ -11729,7 +11761,7 @@
       </c>
       <c r="I269" s="32"/>
     </row>
-    <row r="270" spans="1:9" ht="240">
+    <row r="270" spans="1:9" ht="210">
       <c r="A270" s="30" t="s">
         <v>290</v>
       </c>
@@ -11879,7 +11911,7 @@
       </c>
       <c r="I275" s="32"/>
     </row>
-    <row r="276" spans="1:9" ht="45">
+    <row r="276" spans="1:9" ht="30">
       <c r="A276" s="30" t="s">
         <v>296</v>
       </c>
@@ -11933,7 +11965,7 @@
       </c>
       <c r="I277" s="32"/>
     </row>
-    <row r="278" spans="1:9" ht="30">
+    <row r="278" spans="1:9">
       <c r="A278" s="30" t="s">
         <v>298</v>
       </c>
@@ -12008,7 +12040,7 @@
       </c>
       <c r="I280" s="32"/>
     </row>
-    <row r="281" spans="1:9" ht="30">
+    <row r="281" spans="1:9">
       <c r="A281" s="30" t="s">
         <v>301</v>
       </c>
@@ -12083,7 +12115,7 @@
       </c>
       <c r="I283" s="32"/>
     </row>
-    <row r="284" spans="1:9" ht="30">
+    <row r="284" spans="1:9">
       <c r="A284" s="30" t="s">
         <v>304</v>
       </c>
@@ -12158,7 +12190,7 @@
       </c>
       <c r="I286" s="32"/>
     </row>
-    <row r="287" spans="1:9" ht="45">
+    <row r="287" spans="1:9" ht="30">
       <c r="A287" s="30" t="s">
         <v>307</v>
       </c>
@@ -12208,7 +12240,7 @@
       </c>
       <c r="I288" s="32"/>
     </row>
-    <row r="289" spans="1:9" ht="240">
+    <row r="289" spans="1:9" ht="210">
       <c r="A289" s="30" t="s">
         <v>309</v>
       </c>
@@ -12283,7 +12315,7 @@
       </c>
       <c r="I291" s="32"/>
     </row>
-    <row r="292" spans="1:9" ht="45">
+    <row r="292" spans="1:9" ht="30">
       <c r="A292" s="30" t="s">
         <v>312</v>
       </c>
@@ -12360,7 +12392,7 @@
       </c>
       <c r="I294" s="32"/>
     </row>
-    <row r="295" spans="1:9" ht="30">
+    <row r="295" spans="1:9">
       <c r="A295" s="30" t="s">
         <v>315</v>
       </c>
@@ -12435,7 +12467,7 @@
       </c>
       <c r="I297" s="32"/>
     </row>
-    <row r="298" spans="1:9" ht="30">
+    <row r="298" spans="1:9">
       <c r="A298" s="30" t="s">
         <v>318</v>
       </c>
@@ -12935,7 +12967,7 @@
       </c>
       <c r="I317" s="32"/>
     </row>
-    <row r="318" spans="1:9" ht="30">
+    <row r="318" spans="1:9">
       <c r="A318" s="30" t="s">
         <v>338</v>
       </c>
@@ -13010,7 +13042,7 @@
       </c>
       <c r="I320" s="32"/>
     </row>
-    <row r="321" spans="1:9" ht="135">
+    <row r="321" spans="1:9" ht="120">
       <c r="A321" s="30" t="s">
         <v>341</v>
       </c>
@@ -13035,7 +13067,7 @@
       </c>
       <c r="I321" s="32"/>
     </row>
-    <row r="322" spans="1:9" ht="30">
+    <row r="322" spans="1:9">
       <c r="A322" s="30" t="s">
         <v>342</v>
       </c>
@@ -13085,7 +13117,7 @@
       </c>
       <c r="I323" s="32"/>
     </row>
-    <row r="324" spans="1:9" ht="240">
+    <row r="324" spans="1:9" ht="225">
       <c r="A324" s="30" t="s">
         <v>344</v>
       </c>
@@ -13110,7 +13142,7 @@
       </c>
       <c r="I324" s="32"/>
     </row>
-    <row r="325" spans="1:9" ht="30">
+    <row r="325" spans="1:9">
       <c r="A325" s="30" t="s">
         <v>345</v>
       </c>
@@ -13160,7 +13192,7 @@
       </c>
       <c r="I326" s="32"/>
     </row>
-    <row r="327" spans="1:9" ht="240">
+    <row r="327" spans="1:9" ht="225">
       <c r="A327" s="30" t="s">
         <v>347</v>
       </c>
@@ -13185,7 +13217,7 @@
       </c>
       <c r="I327" s="32"/>
     </row>
-    <row r="328" spans="1:9" ht="30">
+    <row r="328" spans="1:9">
       <c r="A328" s="30" t="s">
         <v>348</v>
       </c>
@@ -13235,7 +13267,7 @@
       </c>
       <c r="I329" s="32"/>
     </row>
-    <row r="330" spans="1:9" ht="240">
+    <row r="330" spans="1:9" ht="225">
       <c r="A330" s="30" t="s">
         <v>350</v>
       </c>
@@ -13260,7 +13292,7 @@
       </c>
       <c r="I330" s="32"/>
     </row>
-    <row r="331" spans="1:9" ht="30">
+    <row r="331" spans="1:9">
       <c r="A331" s="30" t="s">
         <v>351</v>
       </c>
@@ -13310,7 +13342,7 @@
       </c>
       <c r="I332" s="32"/>
     </row>
-    <row r="333" spans="1:9" ht="240">
+    <row r="333" spans="1:9" ht="225">
       <c r="A333" s="30" t="s">
         <v>353</v>
       </c>
@@ -13335,7 +13367,7 @@
       </c>
       <c r="I333" s="32"/>
     </row>
-    <row r="334" spans="1:9" ht="30">
+    <row r="334" spans="1:9">
       <c r="A334" s="30" t="s">
         <v>354</v>
       </c>
@@ -13360,7 +13392,7 @@
       </c>
       <c r="I334" s="32"/>
     </row>
-    <row r="335" spans="1:9" ht="60">
+    <row r="335" spans="1:9" ht="45">
       <c r="A335" s="30" t="s">
         <v>355</v>
       </c>
@@ -13385,7 +13417,7 @@
       </c>
       <c r="I335" s="32"/>
     </row>
-    <row r="336" spans="1:9" ht="240">
+    <row r="336" spans="1:9" ht="225">
       <c r="A336" s="30" t="s">
         <v>356</v>
       </c>
@@ -13460,7 +13492,7 @@
       </c>
       <c r="I338" s="32"/>
     </row>
-    <row r="339" spans="1:9" ht="240">
+    <row r="339" spans="1:9" ht="210">
       <c r="A339" s="30" t="s">
         <v>359</v>
       </c>
@@ -13622,7 +13654,7 @@
         <v>479</v>
       </c>
       <c r="C345" s="32" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D345" s="30" t="s">
         <v>872</v>
@@ -13653,8 +13685,8 @@
       <c r="C346" s="32" t="s">
         <v>881</v>
       </c>
-      <c r="D346" s="30" t="s">
-        <v>883</v>
+      <c r="D346" s="22" t="s">
+        <v>888</v>
       </c>
       <c r="E346" s="30" t="s">
         <v>22</v>
@@ -13682,8 +13714,8 @@
       <c r="C347" s="32" t="s">
         <v>880</v>
       </c>
-      <c r="D347" s="30" t="s">
-        <v>883</v>
+      <c r="D347" s="22" t="s">
+        <v>888</v>
       </c>
       <c r="E347" s="30" t="s">
         <v>22</v>
@@ -13701,7 +13733,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="348" spans="1:9" ht="105">
+    <row r="348" spans="1:9" ht="90">
       <c r="A348" s="30" t="s">
         <v>366</v>
       </c>
@@ -13709,7 +13741,7 @@
         <v>479</v>
       </c>
       <c r="C348" s="32" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D348" s="30"/>
       <c r="E348" s="30" t="s">
@@ -13726,7 +13758,7 @@
       </c>
       <c r="I348" s="32"/>
     </row>
-    <row r="349" spans="1:9" ht="45">
+    <row r="349" spans="1:9" ht="30">
       <c r="A349" s="30" t="s">
         <v>367</v>
       </c>
@@ -13886,7 +13918,7 @@
       </c>
       <c r="I354" s="32"/>
     </row>
-    <row r="355" spans="1:9" ht="195">
+    <row r="355" spans="1:9" ht="135">
       <c r="A355" s="30" t="s">
         <v>373</v>
       </c>
@@ -13911,7 +13943,7 @@
       </c>
       <c r="I355" s="32"/>
     </row>
-    <row r="356" spans="1:9" ht="45">
+    <row r="356" spans="1:9" ht="30">
       <c r="A356" s="30" t="s">
         <v>374</v>
       </c>
@@ -14088,7 +14120,7 @@
       </c>
       <c r="I362" s="32"/>
     </row>
-    <row r="363" spans="1:9" ht="120">
+    <row r="363" spans="1:9" ht="105">
       <c r="A363" s="30" t="s">
         <v>381</v>
       </c>
@@ -14163,7 +14195,7 @@
       </c>
       <c r="I365" s="32"/>
     </row>
-    <row r="366" spans="1:9" ht="165">
+    <row r="366" spans="1:9" ht="135">
       <c r="A366" s="30" t="s">
         <v>384</v>
       </c>
@@ -14313,7 +14345,7 @@
       </c>
       <c r="I371" s="32"/>
     </row>
-    <row r="372" spans="1:9" ht="150">
+    <row r="372" spans="1:9" ht="135">
       <c r="A372" s="30" t="s">
         <v>390</v>
       </c>
@@ -14363,7 +14395,7 @@
       </c>
       <c r="I373" s="32"/>
     </row>
-    <row r="374" spans="1:9" ht="30">
+    <row r="374" spans="1:9">
       <c r="A374" s="30" t="s">
         <v>392</v>
       </c>
@@ -14413,7 +14445,7 @@
       </c>
       <c r="I375" s="32"/>
     </row>
-    <row r="376" spans="1:9" ht="135">
+    <row r="376" spans="1:9" ht="120">
       <c r="A376" s="30" t="s">
         <v>394</v>
       </c>
@@ -14463,7 +14495,7 @@
       </c>
       <c r="I377" s="32"/>
     </row>
-    <row r="378" spans="1:9" ht="120">
+    <row r="378" spans="1:9" ht="105">
       <c r="A378" s="30" t="s">
         <v>396</v>
       </c>
@@ -14498,6 +14530,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -14505,40 +14542,35 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A113:I113 A115:I378 I113:I378 A34:I111 I20:I111 A20:H378">
-    <cfRule type="expression" dxfId="7" priority="53">
+    <cfRule type="expression" dxfId="26" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="54">
+    <cfRule type="expression" dxfId="25" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="61">
+    <cfRule type="expression" dxfId="24" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A113:I113 A115:I378 I113:I378 A34:I111 I20:I111 A20:H378">
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="22" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F378">
-    <cfRule type="expression" dxfId="1" priority="13">
+    <cfRule type="expression" dxfId="20" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="14">
+    <cfRule type="expression" dxfId="19" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14566,7 +14598,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B348:B380 C3 B146:B344 B108:B143 B346 B55:B106 B19:B54" numberStoredAsText="1"/>
+    <ignoredError sqref="B347:B380 C3 B145:B345 B107:B144 B346 B55:B106 B19:B54" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -14625,18 +14657,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14655,6 +14687,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -14666,12 +14706,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>